<commit_message>
Updates to calibration code.
</commit_message>
<xml_diff>
--- a/playback/HINT/HINT (;bandpass;0dB+4talker_ists).xlsx
+++ b/playback/HINT/HINT (;bandpass;0dB+4talker_ists).xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Public\GitHub\SIN\playback\HINT\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="10350"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21576" windowHeight="10356"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2602,7 +2607,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2616,9 +2621,9 @@
       <selection sqref="A1:D279"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2632,7 +2637,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -2646,7 +2651,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -2660,7 +2665,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -2674,7 +2679,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -2688,7 +2693,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -2702,7 +2707,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -2716,7 +2721,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>23</v>
       </c>
@@ -2730,7 +2735,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -2744,7 +2749,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>29</v>
       </c>
@@ -2758,7 +2763,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>32</v>
       </c>
@@ -2772,7 +2777,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>35</v>
       </c>
@@ -2786,7 +2791,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>38</v>
       </c>
@@ -2800,7 +2805,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>41</v>
       </c>
@@ -2814,7 +2819,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>44</v>
       </c>
@@ -2828,7 +2833,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>47</v>
       </c>
@@ -2842,7 +2847,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>50</v>
       </c>
@@ -2856,7 +2861,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>53</v>
       </c>
@@ -2870,7 +2875,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>56</v>
       </c>
@@ -2884,7 +2889,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>59</v>
       </c>
@@ -2898,7 +2903,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>62</v>
       </c>
@@ -2912,7 +2917,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>65</v>
       </c>
@@ -2926,7 +2931,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>68</v>
       </c>
@@ -2940,7 +2945,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>71</v>
       </c>
@@ -2954,7 +2959,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>74</v>
       </c>
@@ -2968,7 +2973,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>77</v>
       </c>
@@ -2982,7 +2987,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>80</v>
       </c>
@@ -2996,7 +3001,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>83</v>
       </c>
@@ -3010,7 +3015,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>86</v>
       </c>
@@ -3024,7 +3029,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>89</v>
       </c>
@@ -3038,7 +3043,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>92</v>
       </c>
@@ -3052,7 +3057,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>95</v>
       </c>
@@ -3066,7 +3071,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>98</v>
       </c>
@@ -3080,7 +3085,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>101</v>
       </c>
@@ -3094,7 +3099,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>104</v>
       </c>
@@ -3108,7 +3113,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>107</v>
       </c>
@@ -3122,7 +3127,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>110</v>
       </c>
@@ -3136,7 +3141,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>113</v>
       </c>
@@ -3150,7 +3155,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>116</v>
       </c>
@@ -3164,7 +3169,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>119</v>
       </c>
@@ -3178,7 +3183,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>122</v>
       </c>
@@ -3192,7 +3197,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>125</v>
       </c>
@@ -3206,7 +3211,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>128</v>
       </c>
@@ -3220,7 +3225,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>131</v>
       </c>
@@ -3234,7 +3239,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>134</v>
       </c>
@@ -3248,7 +3253,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>137</v>
       </c>
@@ -3262,7 +3267,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>140</v>
       </c>
@@ -3276,7 +3281,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>143</v>
       </c>
@@ -3290,7 +3295,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>146</v>
       </c>
@@ -3304,7 +3309,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>149</v>
       </c>
@@ -3318,7 +3323,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>152</v>
       </c>
@@ -3332,7 +3337,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>155</v>
       </c>
@@ -3346,7 +3351,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>158</v>
       </c>
@@ -3360,7 +3365,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>161</v>
       </c>
@@ -3374,7 +3379,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>164</v>
       </c>
@@ -3388,7 +3393,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>167</v>
       </c>
@@ -3402,7 +3407,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>170</v>
       </c>
@@ -3416,7 +3421,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>173</v>
       </c>
@@ -3430,7 +3435,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>176</v>
       </c>
@@ -3444,7 +3449,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>179</v>
       </c>
@@ -3458,7 +3463,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>182</v>
       </c>
@@ -3472,7 +3477,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>185</v>
       </c>
@@ -3486,7 +3491,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>188</v>
       </c>
@@ -3500,7 +3505,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>191</v>
       </c>
@@ -3514,7 +3519,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>194</v>
       </c>
@@ -3528,7 +3533,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>197</v>
       </c>
@@ -3542,7 +3547,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>200</v>
       </c>
@@ -3556,7 +3561,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>203</v>
       </c>
@@ -3570,7 +3575,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>206</v>
       </c>
@@ -3584,7 +3589,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>209</v>
       </c>
@@ -3598,7 +3603,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>212</v>
       </c>
@@ -3612,7 +3617,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>215</v>
       </c>
@@ -3626,7 +3631,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>218</v>
       </c>
@@ -3640,7 +3645,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>221</v>
       </c>
@@ -3654,7 +3659,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>224</v>
       </c>
@@ -3668,7 +3673,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>227</v>
       </c>
@@ -3682,7 +3687,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>230</v>
       </c>
@@ -3696,7 +3701,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>233</v>
       </c>
@@ -3710,7 +3715,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>236</v>
       </c>
@@ -3724,7 +3729,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>239</v>
       </c>
@@ -3738,7 +3743,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>242</v>
       </c>
@@ -3752,7 +3757,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>245</v>
       </c>
@@ -3766,7 +3771,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>248</v>
       </c>
@@ -3780,7 +3785,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>251</v>
       </c>
@@ -3794,7 +3799,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>254</v>
       </c>
@@ -3808,7 +3813,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>257</v>
       </c>
@@ -3822,7 +3827,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>260</v>
       </c>
@@ -3836,7 +3841,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>263</v>
       </c>
@@ -3850,7 +3855,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>266</v>
       </c>
@@ -3864,7 +3869,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>269</v>
       </c>
@@ -3878,7 +3883,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>272</v>
       </c>
@@ -3892,7 +3897,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>275</v>
       </c>
@@ -3906,7 +3911,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>278</v>
       </c>
@@ -3920,7 +3925,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>281</v>
       </c>
@@ -3934,7 +3939,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>284</v>
       </c>
@@ -3948,7 +3953,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>287</v>
       </c>
@@ -3962,7 +3967,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>290</v>
       </c>
@@ -3976,7 +3981,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>293</v>
       </c>
@@ -3990,7 +3995,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>296</v>
       </c>
@@ -4004,7 +4009,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>299</v>
       </c>
@@ -4018,7 +4023,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>302</v>
       </c>
@@ -4032,7 +4037,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>305</v>
       </c>
@@ -4046,7 +4051,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>308</v>
       </c>
@@ -4060,7 +4065,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>311</v>
       </c>
@@ -4074,7 +4079,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>314</v>
       </c>
@@ -4088,7 +4093,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>317</v>
       </c>
@@ -4102,7 +4107,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>320</v>
       </c>
@@ -4116,7 +4121,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>323</v>
       </c>
@@ -4130,7 +4135,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>326</v>
       </c>
@@ -4144,7 +4149,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>329</v>
       </c>
@@ -4158,7 +4163,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>332</v>
       </c>
@@ -4172,7 +4177,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>335</v>
       </c>
@@ -4186,7 +4191,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>338</v>
       </c>
@@ -4200,7 +4205,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>341</v>
       </c>
@@ -4214,7 +4219,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>344</v>
       </c>
@@ -4228,7 +4233,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>347</v>
       </c>
@@ -4242,7 +4247,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>350</v>
       </c>
@@ -4256,7 +4261,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>353</v>
       </c>
@@ -4270,7 +4275,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>356</v>
       </c>
@@ -4284,7 +4289,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>359</v>
       </c>
@@ -4298,7 +4303,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>362</v>
       </c>
@@ -4312,7 +4317,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>365</v>
       </c>
@@ -4326,7 +4331,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>368</v>
       </c>
@@ -4340,7 +4345,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>371</v>
       </c>
@@ -4354,7 +4359,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>374</v>
       </c>
@@ -4368,7 +4373,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>377</v>
       </c>
@@ -4382,7 +4387,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>380</v>
       </c>
@@ -4396,7 +4401,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>383</v>
       </c>
@@ -4410,7 +4415,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>386</v>
       </c>
@@ -4424,7 +4429,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>389</v>
       </c>
@@ -4438,7 +4443,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
         <v>392</v>
       </c>
@@ -4452,7 +4457,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>395</v>
       </c>
@@ -4466,7 +4471,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
         <v>398</v>
       </c>
@@ -4480,7 +4485,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
         <v>401</v>
       </c>
@@ -4494,7 +4499,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>404</v>
       </c>
@@ -4508,7 +4513,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
         <v>407</v>
       </c>
@@ -4522,7 +4527,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
         <v>410</v>
       </c>
@@ -4536,7 +4541,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
         <v>413</v>
       </c>
@@ -4550,7 +4555,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
         <v>416</v>
       </c>
@@ -4564,7 +4569,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
         <v>419</v>
       </c>
@@ -4578,7 +4583,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
         <v>422</v>
       </c>
@@ -4592,7 +4597,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
         <v>425</v>
       </c>
@@ -4606,7 +4611,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
         <v>428</v>
       </c>
@@ -4620,7 +4625,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
         <v>431</v>
       </c>
@@ -4634,7 +4639,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
         <v>434</v>
       </c>
@@ -4648,7 +4653,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
         <v>437</v>
       </c>
@@ -4662,7 +4667,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
         <v>440</v>
       </c>
@@ -4676,7 +4681,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
         <v>443</v>
       </c>
@@ -4690,7 +4695,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
         <v>446</v>
       </c>
@@ -4704,7 +4709,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
         <v>449</v>
       </c>
@@ -4718,7 +4723,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
         <v>452</v>
       </c>
@@ -4732,7 +4737,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
         <v>455</v>
       </c>
@@ -4746,7 +4751,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
         <v>458</v>
       </c>
@@ -4760,7 +4765,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
         <v>461</v>
       </c>
@@ -4774,7 +4779,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
         <v>464</v>
       </c>
@@ -4788,7 +4793,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
         <v>467</v>
       </c>
@@ -4802,7 +4807,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
         <v>470</v>
       </c>
@@ -4816,7 +4821,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
         <v>473</v>
       </c>
@@ -4830,7 +4835,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
         <v>476</v>
       </c>
@@ -4844,7 +4849,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
         <v>479</v>
       </c>
@@ -4858,7 +4863,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
         <v>482</v>
       </c>
@@ -4872,7 +4877,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
         <v>485</v>
       </c>
@@ -4886,7 +4891,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
         <v>488</v>
       </c>
@@ -4900,7 +4905,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
         <v>491</v>
       </c>
@@ -4914,7 +4919,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
         <v>494</v>
       </c>
@@ -4928,7 +4933,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="166" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
         <v>497</v>
       </c>
@@ -4942,7 +4947,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
         <v>500</v>
       </c>
@@ -4956,7 +4961,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
         <v>503</v>
       </c>
@@ -4970,7 +4975,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
         <v>506</v>
       </c>
@@ -4984,7 +4989,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="170" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
         <v>509</v>
       </c>
@@ -4998,7 +5003,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="171" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
         <v>512</v>
       </c>
@@ -5012,7 +5017,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="172" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
         <v>515</v>
       </c>
@@ -5026,7 +5031,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="173" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
         <v>518</v>
       </c>
@@ -5040,7 +5045,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="174" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
         <v>521</v>
       </c>
@@ -5054,7 +5059,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="175" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
         <v>524</v>
       </c>
@@ -5068,7 +5073,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="176" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
         <v>527</v>
       </c>
@@ -5082,7 +5087,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="177" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
         <v>530</v>
       </c>
@@ -5096,7 +5101,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="178" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
         <v>533</v>
       </c>
@@ -5110,7 +5115,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="179" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
         <v>536</v>
       </c>
@@ -5124,7 +5129,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="180" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
         <v>539</v>
       </c>
@@ -5138,7 +5143,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="181" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
         <v>542</v>
       </c>
@@ -5152,7 +5157,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="182" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
         <v>545</v>
       </c>
@@ -5166,7 +5171,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="183" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
         <v>548</v>
       </c>
@@ -5180,7 +5185,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="184" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
         <v>551</v>
       </c>
@@ -5194,7 +5199,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="185" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
         <v>554</v>
       </c>
@@ -5208,7 +5213,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="186" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
         <v>557</v>
       </c>
@@ -5222,7 +5227,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="187" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
         <v>560</v>
       </c>
@@ -5236,7 +5241,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="188" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
         <v>563</v>
       </c>
@@ -5250,7 +5255,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="189" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
         <v>566</v>
       </c>
@@ -5264,7 +5269,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="190" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
         <v>569</v>
       </c>
@@ -5278,7 +5283,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="191" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
         <v>572</v>
       </c>
@@ -5292,7 +5297,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="192" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
         <v>575</v>
       </c>
@@ -5306,7 +5311,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="193" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
         <v>578</v>
       </c>
@@ -5320,7 +5325,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="194" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
         <v>581</v>
       </c>
@@ -5334,7 +5339,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="195" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
         <v>584</v>
       </c>
@@ -5348,7 +5353,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="196" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
         <v>587</v>
       </c>
@@ -5362,7 +5367,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="197" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
         <v>590</v>
       </c>
@@ -5376,7 +5381,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="198" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
         <v>593</v>
       </c>
@@ -5390,7 +5395,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="199" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
         <v>596</v>
       </c>
@@ -5404,7 +5409,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="200" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
         <v>599</v>
       </c>
@@ -5418,7 +5423,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="201" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
         <v>602</v>
       </c>
@@ -5432,7 +5437,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="202" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
         <v>605</v>
       </c>
@@ -5446,7 +5451,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="203" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
         <v>608</v>
       </c>
@@ -5460,7 +5465,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="204" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
         <v>611</v>
       </c>
@@ -5474,7 +5479,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="205" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
         <v>614</v>
       </c>
@@ -5488,7 +5493,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="206" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
         <v>617</v>
       </c>
@@ -5502,7 +5507,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="207" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A207" t="s">
         <v>620</v>
       </c>
@@ -5516,7 +5521,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="208" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A208" t="s">
         <v>623</v>
       </c>
@@ -5530,7 +5535,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="209" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A209" t="s">
         <v>626</v>
       </c>
@@ -5544,7 +5549,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="210" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A210" t="s">
         <v>629</v>
       </c>
@@ -5558,7 +5563,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="211" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A211" t="s">
         <v>632</v>
       </c>
@@ -5572,7 +5577,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="212" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A212" t="s">
         <v>635</v>
       </c>
@@ -5586,7 +5591,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="213" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A213" t="s">
         <v>638</v>
       </c>
@@ -5600,7 +5605,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="214" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A214" t="s">
         <v>641</v>
       </c>
@@ -5614,7 +5619,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="215" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A215" t="s">
         <v>644</v>
       </c>
@@ -5628,7 +5633,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="216" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A216" t="s">
         <v>647</v>
       </c>
@@ -5642,7 +5647,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="217" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A217" t="s">
         <v>650</v>
       </c>
@@ -5656,7 +5661,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="218" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A218" t="s">
         <v>653</v>
       </c>
@@ -5670,7 +5675,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="219" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A219" t="s">
         <v>656</v>
       </c>
@@ -5684,7 +5689,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="220" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A220" t="s">
         <v>659</v>
       </c>
@@ -5698,7 +5703,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="221" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A221" t="s">
         <v>662</v>
       </c>
@@ -5712,7 +5717,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="222" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A222" t="s">
         <v>665</v>
       </c>
@@ -5726,7 +5731,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="223" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A223" t="s">
         <v>668</v>
       </c>
@@ -5740,7 +5745,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="224" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A224" t="s">
         <v>671</v>
       </c>
@@ -5754,7 +5759,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="225" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A225" t="s">
         <v>674</v>
       </c>
@@ -5768,7 +5773,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="226" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A226" t="s">
         <v>677</v>
       </c>
@@ -5782,7 +5787,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="227" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A227" t="s">
         <v>680</v>
       </c>
@@ -5796,7 +5801,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="228" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A228" t="s">
         <v>683</v>
       </c>
@@ -5810,7 +5815,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="229" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A229" t="s">
         <v>686</v>
       </c>
@@ -5824,7 +5829,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="230" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A230" t="s">
         <v>689</v>
       </c>
@@ -5838,7 +5843,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="231" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A231" t="s">
         <v>692</v>
       </c>
@@ -5852,7 +5857,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="232" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A232" t="s">
         <v>695</v>
       </c>
@@ -5866,7 +5871,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="233" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A233" t="s">
         <v>698</v>
       </c>
@@ -5880,7 +5885,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="234" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A234" t="s">
         <v>701</v>
       </c>
@@ -5894,7 +5899,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="235" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A235" t="s">
         <v>704</v>
       </c>
@@ -5908,7 +5913,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="236" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A236" t="s">
         <v>707</v>
       </c>
@@ -5922,7 +5927,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="237" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A237" t="s">
         <v>710</v>
       </c>
@@ -5936,7 +5941,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="238" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A238" t="s">
         <v>713</v>
       </c>
@@ -5950,7 +5955,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="239" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A239" t="s">
         <v>716</v>
       </c>
@@ -5964,7 +5969,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="240" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A240" t="s">
         <v>719</v>
       </c>
@@ -5978,7 +5983,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="241" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A241" t="s">
         <v>722</v>
       </c>
@@ -5992,7 +5997,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="242" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A242" t="s">
         <v>725</v>
       </c>
@@ -6006,7 +6011,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="243" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A243" t="s">
         <v>728</v>
       </c>
@@ -6020,7 +6025,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="244" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A244" t="s">
         <v>731</v>
       </c>
@@ -6034,7 +6039,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="245" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A245" t="s">
         <v>734</v>
       </c>
@@ -6048,7 +6053,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="246" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A246" t="s">
         <v>737</v>
       </c>
@@ -6062,7 +6067,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="247" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A247" t="s">
         <v>740</v>
       </c>
@@ -6076,7 +6081,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="248" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A248" t="s">
         <v>743</v>
       </c>
@@ -6090,7 +6095,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="249" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A249" t="s">
         <v>746</v>
       </c>
@@ -6104,7 +6109,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="250" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A250" t="s">
         <v>749</v>
       </c>
@@ -6118,7 +6123,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="251" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A251" t="s">
         <v>752</v>
       </c>
@@ -6132,7 +6137,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="252" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A252" t="s">
         <v>755</v>
       </c>

</xml_diff>

<commit_message>
Updates to lookup tables and make_stimuli routine.
</commit_message>
<xml_diff>
--- a/playback/HINT/HINT (;bandpass;0dB+4talker_ists).xlsx
+++ b/playback/HINT/HINT (;bandpass;0dB+4talker_ists).xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Public\GitHub\SIN\playback\HINT\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21576" windowHeight="10356"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="10350"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2607,7 +2602,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2621,9 +2616,9 @@
       <selection sqref="A1:D279"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2637,7 +2632,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -2651,7 +2646,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -2665,7 +2660,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -2679,7 +2674,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -2693,7 +2688,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -2707,7 +2702,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -2721,7 +2716,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>23</v>
       </c>
@@ -2735,7 +2730,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -2749,7 +2744,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>29</v>
       </c>
@@ -2763,7 +2758,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>32</v>
       </c>
@@ -2777,7 +2772,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>35</v>
       </c>
@@ -2791,7 +2786,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>38</v>
       </c>
@@ -2805,7 +2800,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>41</v>
       </c>
@@ -2819,7 +2814,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>44</v>
       </c>
@@ -2833,7 +2828,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>47</v>
       </c>
@@ -2847,7 +2842,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>50</v>
       </c>
@@ -2861,7 +2856,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>53</v>
       </c>
@@ -2875,7 +2870,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>56</v>
       </c>
@@ -2889,7 +2884,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>59</v>
       </c>
@@ -2903,7 +2898,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>62</v>
       </c>
@@ -2917,7 +2912,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>65</v>
       </c>
@@ -2931,7 +2926,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>68</v>
       </c>
@@ -2945,7 +2940,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>71</v>
       </c>
@@ -2959,7 +2954,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>74</v>
       </c>
@@ -2973,7 +2968,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>77</v>
       </c>
@@ -2987,7 +2982,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>80</v>
       </c>
@@ -3001,7 +2996,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>83</v>
       </c>
@@ -3015,7 +3010,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>86</v>
       </c>
@@ -3029,7 +3024,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>89</v>
       </c>
@@ -3043,7 +3038,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>92</v>
       </c>
@@ -3057,7 +3052,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>95</v>
       </c>
@@ -3071,7 +3066,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>98</v>
       </c>
@@ -3085,7 +3080,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>101</v>
       </c>
@@ -3099,7 +3094,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>104</v>
       </c>
@@ -3113,7 +3108,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>107</v>
       </c>
@@ -3127,7 +3122,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>110</v>
       </c>
@@ -3141,7 +3136,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>113</v>
       </c>
@@ -3155,7 +3150,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>116</v>
       </c>
@@ -3169,7 +3164,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>119</v>
       </c>
@@ -3183,7 +3178,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>122</v>
       </c>
@@ -3197,7 +3192,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>125</v>
       </c>
@@ -3211,7 +3206,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>128</v>
       </c>
@@ -3225,7 +3220,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>131</v>
       </c>
@@ -3239,7 +3234,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>134</v>
       </c>
@@ -3253,7 +3248,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>137</v>
       </c>
@@ -3267,7 +3262,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>140</v>
       </c>
@@ -3281,7 +3276,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>143</v>
       </c>
@@ -3295,7 +3290,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>146</v>
       </c>
@@ -3309,7 +3304,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>149</v>
       </c>
@@ -3323,7 +3318,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>152</v>
       </c>
@@ -3337,7 +3332,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>155</v>
       </c>
@@ -3351,7 +3346,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>158</v>
       </c>
@@ -3365,7 +3360,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>161</v>
       </c>
@@ -3379,7 +3374,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>164</v>
       </c>
@@ -3393,7 +3388,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>167</v>
       </c>
@@ -3407,7 +3402,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>170</v>
       </c>
@@ -3421,7 +3416,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>173</v>
       </c>
@@ -3435,7 +3430,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>176</v>
       </c>
@@ -3449,7 +3444,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>179</v>
       </c>
@@ -3463,7 +3458,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>182</v>
       </c>
@@ -3477,7 +3472,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>185</v>
       </c>
@@ -3491,7 +3486,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>188</v>
       </c>
@@ -3505,7 +3500,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>191</v>
       </c>
@@ -3519,7 +3514,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>194</v>
       </c>
@@ -3533,7 +3528,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>197</v>
       </c>
@@ -3547,7 +3542,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>200</v>
       </c>
@@ -3561,7 +3556,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>203</v>
       </c>
@@ -3575,7 +3570,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>206</v>
       </c>
@@ -3589,7 +3584,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>209</v>
       </c>
@@ -3603,7 +3598,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>212</v>
       </c>
@@ -3617,7 +3612,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>215</v>
       </c>
@@ -3631,7 +3626,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>218</v>
       </c>
@@ -3645,7 +3640,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>221</v>
       </c>
@@ -3659,7 +3654,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>224</v>
       </c>
@@ -3673,7 +3668,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>227</v>
       </c>
@@ -3687,7 +3682,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>230</v>
       </c>
@@ -3701,7 +3696,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>233</v>
       </c>
@@ -3715,7 +3710,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>236</v>
       </c>
@@ -3729,7 +3724,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>239</v>
       </c>
@@ -3743,7 +3738,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>242</v>
       </c>
@@ -3757,7 +3752,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>245</v>
       </c>
@@ -3771,7 +3766,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>248</v>
       </c>
@@ -3785,7 +3780,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>251</v>
       </c>
@@ -3799,7 +3794,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>254</v>
       </c>
@@ -3813,7 +3808,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>257</v>
       </c>
@@ -3827,7 +3822,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>260</v>
       </c>
@@ -3841,7 +3836,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>263</v>
       </c>
@@ -3855,7 +3850,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>266</v>
       </c>
@@ -3869,7 +3864,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>269</v>
       </c>
@@ -3883,7 +3878,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>272</v>
       </c>
@@ -3897,7 +3892,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>275</v>
       </c>
@@ -3911,7 +3906,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>278</v>
       </c>
@@ -3925,7 +3920,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>281</v>
       </c>
@@ -3939,7 +3934,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>284</v>
       </c>
@@ -3953,7 +3948,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>287</v>
       </c>
@@ -3967,7 +3962,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>290</v>
       </c>
@@ -3981,7 +3976,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>293</v>
       </c>
@@ -3995,7 +3990,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>296</v>
       </c>
@@ -4009,7 +4004,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>299</v>
       </c>
@@ -4023,7 +4018,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>302</v>
       </c>
@@ -4037,7 +4032,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>305</v>
       </c>
@@ -4051,7 +4046,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>308</v>
       </c>
@@ -4065,7 +4060,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>311</v>
       </c>
@@ -4079,7 +4074,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>314</v>
       </c>
@@ -4093,7 +4088,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>317</v>
       </c>
@@ -4107,7 +4102,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>320</v>
       </c>
@@ -4121,7 +4116,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>323</v>
       </c>
@@ -4135,7 +4130,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>326</v>
       </c>
@@ -4149,7 +4144,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>329</v>
       </c>
@@ -4163,7 +4158,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>332</v>
       </c>
@@ -4177,7 +4172,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>335</v>
       </c>
@@ -4191,7 +4186,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>338</v>
       </c>
@@ -4205,7 +4200,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>341</v>
       </c>
@@ -4219,7 +4214,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>344</v>
       </c>
@@ -4233,7 +4228,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>347</v>
       </c>
@@ -4247,7 +4242,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>350</v>
       </c>
@@ -4261,7 +4256,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>353</v>
       </c>
@@ -4275,7 +4270,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>356</v>
       </c>
@@ -4289,7 +4284,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>359</v>
       </c>
@@ -4303,7 +4298,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>362</v>
       </c>
@@ -4317,7 +4312,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>365</v>
       </c>
@@ -4331,7 +4326,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>368</v>
       </c>
@@ -4345,7 +4340,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>371</v>
       </c>
@@ -4359,7 +4354,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>374</v>
       </c>
@@ -4373,7 +4368,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>377</v>
       </c>
@@ -4387,7 +4382,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>380</v>
       </c>
@@ -4401,7 +4396,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>383</v>
       </c>
@@ -4415,7 +4410,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>386</v>
       </c>
@@ -4429,7 +4424,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>389</v>
       </c>
@@ -4443,7 +4438,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>392</v>
       </c>
@@ -4457,7 +4452,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>395</v>
       </c>
@@ -4471,7 +4466,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>398</v>
       </c>
@@ -4485,7 +4480,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>401</v>
       </c>
@@ -4499,7 +4494,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>404</v>
       </c>
@@ -4513,7 +4508,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>407</v>
       </c>
@@ -4527,7 +4522,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>410</v>
       </c>
@@ -4541,7 +4536,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>413</v>
       </c>
@@ -4555,7 +4550,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>416</v>
       </c>
@@ -4569,7 +4564,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>419</v>
       </c>
@@ -4583,7 +4578,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>422</v>
       </c>
@@ -4597,7 +4592,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>425</v>
       </c>
@@ -4611,7 +4606,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>428</v>
       </c>
@@ -4625,7 +4620,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>431</v>
       </c>
@@ -4639,7 +4634,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>434</v>
       </c>
@@ -4653,7 +4648,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>437</v>
       </c>
@@ -4667,7 +4662,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>440</v>
       </c>
@@ -4681,7 +4676,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>443</v>
       </c>
@@ -4695,7 +4690,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>446</v>
       </c>
@@ -4709,7 +4704,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>449</v>
       </c>
@@ -4723,7 +4718,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>452</v>
       </c>
@@ -4737,7 +4732,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>455</v>
       </c>
@@ -4751,7 +4746,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>458</v>
       </c>
@@ -4765,7 +4760,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>461</v>
       </c>
@@ -4779,7 +4774,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>464</v>
       </c>
@@ -4793,7 +4788,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>467</v>
       </c>
@@ -4807,7 +4802,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>470</v>
       </c>
@@ -4821,7 +4816,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>473</v>
       </c>
@@ -4835,7 +4830,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>476</v>
       </c>
@@ -4849,7 +4844,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>479</v>
       </c>
@@ -4863,7 +4858,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="161" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>482</v>
       </c>
@@ -4877,7 +4872,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="162" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>485</v>
       </c>
@@ -4891,7 +4886,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="163" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>488</v>
       </c>
@@ -4905,7 +4900,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="164" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>491</v>
       </c>
@@ -4919,7 +4914,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="165" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>494</v>
       </c>
@@ -4933,7 +4928,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="166" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>497</v>
       </c>
@@ -4947,7 +4942,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="167" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>500</v>
       </c>
@@ -4961,7 +4956,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="168" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>503</v>
       </c>
@@ -4975,7 +4970,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="169" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>506</v>
       </c>
@@ -4989,7 +4984,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="170" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>509</v>
       </c>
@@ -5003,7 +4998,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="171" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>512</v>
       </c>
@@ -5017,7 +5012,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="172" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>515</v>
       </c>
@@ -5031,7 +5026,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="173" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>518</v>
       </c>
@@ -5045,7 +5040,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="174" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>521</v>
       </c>
@@ -5059,7 +5054,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="175" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>524</v>
       </c>
@@ -5073,7 +5068,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="176" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>527</v>
       </c>
@@ -5087,7 +5082,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="177" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>530</v>
       </c>
@@ -5101,7 +5096,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="178" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>533</v>
       </c>
@@ -5115,7 +5110,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="179" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>536</v>
       </c>
@@ -5129,7 +5124,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="180" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>539</v>
       </c>
@@ -5143,7 +5138,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="181" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>542</v>
       </c>
@@ -5157,7 +5152,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="182" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>545</v>
       </c>
@@ -5171,7 +5166,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="183" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>548</v>
       </c>
@@ -5185,7 +5180,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="184" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>551</v>
       </c>
@@ -5199,7 +5194,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="185" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>554</v>
       </c>
@@ -5213,7 +5208,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="186" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>557</v>
       </c>
@@ -5227,7 +5222,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="187" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>560</v>
       </c>
@@ -5241,7 +5236,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="188" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>563</v>
       </c>
@@ -5255,7 +5250,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="189" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>566</v>
       </c>
@@ -5269,7 +5264,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="190" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>569</v>
       </c>
@@ -5283,7 +5278,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="191" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>572</v>
       </c>
@@ -5297,7 +5292,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="192" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>575</v>
       </c>
@@ -5311,7 +5306,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="193" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>578</v>
       </c>
@@ -5325,7 +5320,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="194" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>581</v>
       </c>
@@ -5339,7 +5334,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="195" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>584</v>
       </c>
@@ -5353,7 +5348,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="196" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>587</v>
       </c>
@@ -5367,7 +5362,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="197" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>590</v>
       </c>
@@ -5381,7 +5376,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="198" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>593</v>
       </c>
@@ -5395,7 +5390,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="199" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>596</v>
       </c>
@@ -5409,7 +5404,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="200" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>599</v>
       </c>
@@ -5423,7 +5418,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="201" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>602</v>
       </c>
@@ -5437,7 +5432,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="202" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
         <v>605</v>
       </c>
@@ -5451,7 +5446,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="203" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>608</v>
       </c>
@@ -5465,7 +5460,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="204" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>611</v>
       </c>
@@ -5479,7 +5474,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="205" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>614</v>
       </c>
@@ -5493,7 +5488,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="206" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>617</v>
       </c>
@@ -5507,7 +5502,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="207" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>620</v>
       </c>
@@ -5521,7 +5516,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="208" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
         <v>623</v>
       </c>
@@ -5535,7 +5530,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="209" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>626</v>
       </c>
@@ -5549,7 +5544,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="210" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>629</v>
       </c>
@@ -5563,7 +5558,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="211" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
         <v>632</v>
       </c>
@@ -5577,7 +5572,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="212" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
         <v>635</v>
       </c>
@@ -5591,7 +5586,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="213" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
         <v>638</v>
       </c>
@@ -5605,7 +5600,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="214" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
         <v>641</v>
       </c>
@@ -5619,7 +5614,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="215" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
         <v>644</v>
       </c>
@@ -5633,7 +5628,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="216" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
         <v>647</v>
       </c>
@@ -5647,7 +5642,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="217" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
         <v>650</v>
       </c>
@@ -5661,7 +5656,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="218" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
         <v>653</v>
       </c>
@@ -5675,7 +5670,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="219" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
         <v>656</v>
       </c>
@@ -5689,7 +5684,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="220" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
         <v>659</v>
       </c>
@@ -5703,7 +5698,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="221" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
         <v>662</v>
       </c>
@@ -5717,7 +5712,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="222" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
         <v>665</v>
       </c>
@@ -5731,7 +5726,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="223" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
         <v>668</v>
       </c>
@@ -5745,7 +5740,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="224" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
         <v>671</v>
       </c>
@@ -5759,7 +5754,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="225" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
         <v>674</v>
       </c>
@@ -5773,7 +5768,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="226" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
         <v>677</v>
       </c>
@@ -5787,7 +5782,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="227" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
         <v>680</v>
       </c>
@@ -5801,7 +5796,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="228" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
         <v>683</v>
       </c>
@@ -5815,7 +5810,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="229" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
         <v>686</v>
       </c>
@@ -5829,7 +5824,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="230" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
         <v>689</v>
       </c>
@@ -5843,7 +5838,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="231" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
         <v>692</v>
       </c>
@@ -5857,7 +5852,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="232" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
         <v>695</v>
       </c>
@@ -5871,7 +5866,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="233" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
         <v>698</v>
       </c>
@@ -5885,7 +5880,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="234" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
         <v>701</v>
       </c>
@@ -5899,7 +5894,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="235" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
         <v>704</v>
       </c>
@@ -5913,7 +5908,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="236" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
         <v>707</v>
       </c>
@@ -5927,7 +5922,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="237" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
         <v>710</v>
       </c>
@@ -5941,7 +5936,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="238" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
         <v>713</v>
       </c>
@@ -5955,7 +5950,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="239" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
         <v>716</v>
       </c>
@@ -5969,7 +5964,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="240" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
         <v>719</v>
       </c>
@@ -5983,7 +5978,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="241" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
         <v>722</v>
       </c>
@@ -5997,7 +5992,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="242" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
         <v>725</v>
       </c>
@@ -6011,7 +6006,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="243" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
         <v>728</v>
       </c>
@@ -6025,7 +6020,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="244" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
         <v>731</v>
       </c>
@@ -6039,7 +6034,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="245" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
         <v>734</v>
       </c>
@@ -6053,7 +6048,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="246" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
         <v>737</v>
       </c>
@@ -6067,7 +6062,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="247" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
         <v>740</v>
       </c>
@@ -6081,7 +6076,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="248" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
         <v>743</v>
       </c>
@@ -6095,7 +6090,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="249" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
         <v>746</v>
       </c>
@@ -6109,7 +6104,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="250" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
         <v>749</v>
       </c>
@@ -6123,7 +6118,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="251" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
         <v>752</v>
       </c>
@@ -6137,7 +6132,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="252" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
         <v>755</v>
       </c>

</xml_diff>